<commit_message>
2 ajouts de billets
</commit_message>
<xml_diff>
--- a/Billets.xlsx
+++ b/Billets.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="105" windowWidth="28515" windowHeight="14580"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="49">
   <si>
     <t>Statut</t>
   </si>
@@ -139,6 +139,30 @@
   </si>
   <si>
     <t>Bonus 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 13-02-2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 13-02-2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 13-02-2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 14-02-2018</t>
+  </si>
+  <si>
+    <t>Icon</t>
+  </si>
+  <si>
+    <t>L'icon de l'app qui apparait est l'icon par defaut</t>
+  </si>
+  <si>
+    <t>Chronomètre ne recommance pas a chaque fois qu'on entre un mot</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 14-02-2019</t>
   </si>
 </sst>
 </file>
@@ -307,13 +331,13 @@
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="20 % - Accent2" xfId="5" builtinId="34"/>
-    <cellStyle name="20 % - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="Calcul" xfId="4" builtinId="22"/>
-    <cellStyle name="Insatisfaisant" xfId="2" builtinId="27"/>
-    <cellStyle name="Neutre" xfId="3" builtinId="28"/>
+    <cellStyle name="20% - Accent2" xfId="5" builtinId="34"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Calculation" xfId="4" builtinId="22"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Satisfaisant" xfId="1" builtinId="26"/>
   </cellStyles>
   <dxfs count="9">
     <dxf>
@@ -326,7 +350,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFB4413E"/>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCC00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -340,14 +371,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
+          <bgColor rgb="FFB4413E"/>
         </patternFill>
       </fill>
     </dxf>
@@ -400,7 +424,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -689,16 +713,16 @@
   <dimension ref="A3:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="27.42578125" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="21.28515625" customWidth="1"/>
     <col min="5" max="5" width="19.42578125" customWidth="1"/>
-    <col min="6" max="6" width="55.85546875" customWidth="1"/>
+    <col min="6" max="6" width="63.85546875" customWidth="1"/>
     <col min="7" max="7" width="20.85546875" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" customWidth="1"/>
     <col min="10" max="10" width="14.7109375" customWidth="1"/>
@@ -978,9 +1002,15 @@
       <c r="C13" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
+      <c r="D13" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>46</v>
+      </c>
       <c r="G13" s="7" t="s">
         <v>17</v>
       </c>
@@ -998,9 +1028,15 @@
       <c r="C14" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
+      <c r="D14" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>47</v>
+      </c>
       <c r="G14" s="7" t="s">
         <v>17</v>
       </c>
@@ -1018,7 +1054,9 @@
       <c r="C15" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="7"/>
+      <c r="D15" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7" t="s">
@@ -1038,7 +1076,9 @@
       <c r="C16" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="7"/>
+      <c r="D16" s="7" t="s">
+        <v>42</v>
+      </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7" t="s">
@@ -1058,7 +1098,9 @@
       <c r="C17" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="7"/>
+      <c r="D17" s="7" t="s">
+        <v>43</v>
+      </c>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7" t="s">
@@ -1084,16 +1126,16 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:G17">
-    <cfRule type="cellIs" dxfId="1" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
       <formula>"Critique"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
       <formula>"Élevé"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"Moyen"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Bas"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
@@ -1137,7 +1179,7 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="28.28515625" customWidth="1"/>
     <col min="3" max="3" width="28.5703125" customWidth="1"/>
@@ -1209,7 +1251,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>